<commit_message>
feat: added support simple lists
</commit_message>
<xml_diff>
--- a/test/simple.xlsx
+++ b/test/simple.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27109"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED4E241D-E08E-469E-AFC9-E5117A622A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{997F9485-0ED6-44E9-9D8A-0FD7DDDC88D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -206,7 +206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -364,11 +364,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -403,9 +429,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -415,9 +438,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -436,7 +456,17 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -753,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G18" sqref="G5:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -769,7 +799,7 @@
     <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -779,7 +809,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="27">
+    <row r="2" spans="1:7" ht="27">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -791,7 +821,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
@@ -803,7 +833,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -815,173 +845,187 @@
       <c r="E4" s="6"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5" s="22"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6" s="22"/>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="13" t="s">
+      <c r="F7" s="22"/>
+      <c r="G7" s="21"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="13" t="s">
+      <c r="F8" s="22"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="13" t="s">
+      <c r="F9" s="22"/>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="13" t="s">
+      <c r="F10" s="22"/>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="13" t="s">
+      <c r="F11" s="22"/>
+      <c r="G11" s="21"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="F12" s="22"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="15"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="17" t="s">
+      <c r="F13" s="22"/>
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="14"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="21"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="21"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="19" t="e">
+      <c r="D16" s="17" t="e">
         <f>C16-B16</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="17">
         <v>10</v>
       </c>
-      <c r="F16" s="12" t="e">
+      <c r="F16" s="22" t="e">
         <f>E16*D16*24</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="15"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75">
-      <c r="A18" s="15"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="20" t="s">
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="14"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75">
+      <c r="A18" s="14"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="21" t="e">
+      <c r="D18" s="19" t="e">
         <f>SUM(D16:D17)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="23" t="e">
+      <c r="F18" s="25" t="e">
         <f>SUM(F16:F17)</f>
         <v>#VALUE!</v>
       </c>
+      <c r="G18" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>